<commit_message>
added entities to input file min.xlsx; added min_building
</commit_message>
<xml_diff>
--- a/data/min/min.xlsx
+++ b/data/min/min.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Commodity" sheetId="1" r:id="rId1"/>
-    <sheet name="Process" sheetId="2" r:id="rId2"/>
-    <sheet name="Process-Commodity" sheetId="3" r:id="rId3"/>
-    <sheet name="Storage" sheetId="4" r:id="rId4"/>
-    <sheet name="Time" sheetId="5" r:id="rId5"/>
+    <sheet name="Readme" sheetId="6" r:id="rId1"/>
+    <sheet name="Commodity" sheetId="1" r:id="rId2"/>
+    <sheet name="Process" sheetId="2" r:id="rId3"/>
+    <sheet name="Process-Commodity" sheetId="9" r:id="rId4"/>
+    <sheet name="Storage" sheetId="4" r:id="rId5"/>
+    <sheet name="Time" sheetId="5" r:id="rId6"/>
+    <sheet name="Area-Demand" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="67">
   <si>
     <t>Commodity</t>
   </si>
@@ -126,16 +128,180 @@
   </si>
   <si>
     <t>peak</t>
+  </si>
+  <si>
+    <t>loss-fix</t>
+  </si>
+  <si>
+    <t>loss-var</t>
+  </si>
+  <si>
+    <t>CAPMIN</t>
+  </si>
+  <si>
+    <t>Optimize urban energy infrastructure with MILP</t>
+  </si>
+  <si>
+    <t>This file contains all non-spatial data that can/should be entered by hand. These are:</t>
+  </si>
+  <si>
+    <t>- Commodity</t>
+  </si>
+  <si>
+    <t>- Process</t>
+  </si>
+  <si>
+    <t>- Process-Commodity</t>
+  </si>
+  <si>
+    <t>- Storage</t>
+  </si>
+  <si>
+    <t>- Time</t>
+  </si>
+  <si>
+    <t>- Vertices</t>
+  </si>
+  <si>
+    <t>- Edges</t>
+  </si>
+  <si>
+    <t>- Buildings</t>
+  </si>
+  <si>
+    <t>- Building</t>
+  </si>
+  <si>
+    <t>all goods in this model: Elect, Heat, Gas, Cool, CO2</t>
+  </si>
+  <si>
+    <t>commodity-converters: general parameters</t>
+  </si>
+  <si>
+    <t>mapping: input/output commodities to processes</t>
+  </si>
+  <si>
+    <t>(unused): storage technologies</t>
+  </si>
+  <si>
+    <t>timestep length (=weight) and height</t>
+  </si>
+  <si>
+    <t>area-specific peak and annual demand for commodity</t>
+  </si>
+  <si>
+    <t>Spatial data, each saved in its individual shapefile:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">location for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commodity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> input and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>processes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">length, aggregated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">building areas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>determine demand</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">area, type: is aggregated to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>edges</t>
+    </r>
+  </si>
+  <si>
+    <t>residential</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Power plant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +309,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +385,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -184,27 +400,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="5">
     <dxf>
       <border>
         <top style="thin">
@@ -213,30 +540,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <border>
@@ -255,6 +558,12 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -558,9 +867,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+      <c r="C8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="22"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -571,88 +1249,128 @@
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="11.42578125" style="8"/>
-    <col min="4" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="11.42578125" style="7"/>
+    <col min="4" max="5" width="11.42578125" style="11"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="11">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="11">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1.6000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="e">
+      <c r="C6" s="7" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="D6" s="11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="2" priority="1">
+    <cfRule type="containsErrors" dxfId="4" priority="1">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -665,7 +1383,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -718,21 +1436,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="11.42578125" style="6"/>
+    <col min="4" max="4" width="11.42578125" style="9"/>
     <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -746,7 +1464,7 @@
       <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -760,7 +1478,7 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="9">
         <v>1</v>
       </c>
     </row>
@@ -774,7 +1492,7 @@
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="9">
         <v>0.3</v>
       </c>
     </row>
@@ -788,7 +1506,7 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="9">
         <v>0.7</v>
       </c>
     </row>
@@ -802,7 +1520,7 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="9">
         <v>0.02</v>
       </c>
     </row>
@@ -816,7 +1534,7 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
     </row>
@@ -830,7 +1548,7 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="9">
         <v>0.3</v>
       </c>
     </row>
@@ -844,7 +1562,7 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="9">
         <v>0.7</v>
       </c>
     </row>
@@ -853,12 +1571,12 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="9">
         <v>0.02</v>
       </c>
     </row>
@@ -872,7 +1590,7 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
     </row>
@@ -886,8 +1604,50 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -900,16 +1660,16 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{02916CE4-83B1-441A-9409-E4C7D1958D6A}</x14:id>
+          <x14:id>{D878AEE9-6E97-4D8E-BFD7-E9DCD820210D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -919,7 +1679,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{02916CE4-83B1-441A-9409-E4C7D1958D6A}">
+          <x14:cfRule type="dataBar" id="{D878AEE9-6E97-4D8E-BFD7-E9DCD820210D}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="num">
@@ -937,7 +1697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1097,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1110,9 +1870,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="11.42578125" style="9"/>
     <col min="4" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -1123,7 +1883,7 @@
       <c r="B1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1131,10 +1891,10 @@
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1142,10 +1902,10 @@
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0.25</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>0.75</v>
       </c>
     </row>
@@ -1153,10 +1913,10 @@
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.5</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.4</v>
       </c>
     </row>
@@ -1164,14 +1924,226 @@
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.25</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="35"/>
+    <col min="4" max="4" width="11.42578125" style="33"/>
+    <col min="5" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="35">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D2" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="33">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="D4" s="33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="35">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D5" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="D7" s="33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="35">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="D10" s="33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="35">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="D13" s="33">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed min example data
</commit_message>
<xml_diff>
--- a/data/min/min.xlsx
+++ b/data/min/min.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>Commodity</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>mapping: input/output commodities to processes</t>
-  </si>
-  <si>
-    <t>(unused): storage technologies</t>
   </si>
   <si>
     <t>timestep length (=weight) and height</t>
@@ -204,22 +201,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>determine demand</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">area, type: is aggregated to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="6" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>edges</t>
     </r>
   </si>
   <si>
@@ -304,6 +285,25 @@
   </si>
   <si>
     <t>cap-installed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">area, type, nearest edge ID: is aggregated to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>edges</t>
+    </r>
+  </si>
+  <si>
+    <t>(unused for now): storage technologies</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -541,6 +541,15 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -556,12 +565,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color theme="0" tint="-0.499984740745262"/>
@@ -569,6 +572,12 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -875,7 +884,7 @@
   <dimension ref="B2:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +920,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -946,7 +955,7 @@
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -1008,7 +1017,7 @@
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="13"/>
@@ -1023,7 +1032,7 @@
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1038,7 +1047,7 @@
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1060,7 +1069,7 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1077,7 +1086,7 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1092,7 +1101,7 @@
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -1107,7 +1116,7 @@
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -1244,125 +1253,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="11.42578125" style="7"/>
-    <col min="4" max="5" width="11.42578125" style="11"/>
-    <col min="6" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="4" width="11.42578125" style="3"/>
+    <col min="5" max="5" width="11.42578125" style="7"/>
+    <col min="6" max="7" width="11.42578125" style="11"/>
+    <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>0.3</v>
       </c>
-      <c r="D2" s="11">
+      <c r="F2" s="11">
         <v>0.01</v>
       </c>
-      <c r="E2" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
         <v>0.6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="F3" s="11">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D4" s="11">
+      <c r="F4" s="11">
         <v>10</v>
       </c>
-      <c r="E4" s="11">
+      <c r="G4" s="11">
         <v>2.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="3">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
         <v>0.08</v>
       </c>
-      <c r="D5" s="11">
+      <c r="F5" s="11">
         <v>8</v>
       </c>
-      <c r="E5" s="11">
+      <c r="G5" s="11">
         <v>1.6000000000000001E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="e">
+      <c r="C6" s="36" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="D6" s="11" t="e">
+      <c r="D6" s="36" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="11" t="e">
+      <c r="E6" s="37" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="38" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="38" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="36" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1380,24 +1446,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="3"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="4" width="11.42578125" style="3"/>
+    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1408,16 +1474,19 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1431,13 +1500,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
         <v>100</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1451,13 +1523,16 @@
         <v>0</v>
       </c>
       <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
         <v>100</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1474,12 +1549,15 @@
         <v>0</v>
       </c>
       <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
         <v>8000</v>
@@ -1489,6 +1567,15 @@
       </c>
       <c r="D5" s="3">
         <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1757,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -1684,7 +1771,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -1698,7 +1785,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -1726,10 +1813,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1971,7 +2058,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="5">
         <v>0.5</v>
@@ -2004,7 +2091,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,7 +2104,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2026,12 +2113,12 @@
         <v>34</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -2045,7 +2132,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2059,7 +2146,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -2073,7 +2160,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -2087,7 +2174,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -2101,7 +2188,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -2115,7 +2202,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -2129,7 +2216,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -2143,7 +2230,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -2157,7 +2244,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
@@ -2171,7 +2258,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -2185,7 +2272,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -2199,7 +2286,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>